<commit_message>
Cleanup excel read code
</commit_message>
<xml_diff>
--- a/Other/ScorecardData.xlsx
+++ b/Other/ScorecardData.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcsiple/Dropbox/Fun Side Projects/ScorecardApp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcsiple/Dropbox/TidyTuesday/Other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9517B26C-0161-7449-8558-60E1F04D8DE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E06173-3313-DD45-BE72-9399E66B98FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="1640" windowWidth="22340" windowHeight="15420" activeTab="1" xr2:uid="{550D27AC-50D2-1E40-A168-D2C463731F4D}"/>
+    <workbookView xWindow="5700" yWindow="1880" windowWidth="22340" windowHeight="15420" activeTab="1" xr2:uid="{550D27AC-50D2-1E40-A168-D2C463731F4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Scores" sheetId="1" r:id="rId1"/>
-    <sheet name="ScorecardInfo" sheetId="2" r:id="rId2"/>
+    <sheet name="Scores_num" sheetId="3" r:id="rId2"/>
+    <sheet name="ScorecardInfo" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
   <si>
     <t>Sunrise</t>
   </si>
@@ -501,7 +502,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection sqref="A1:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -723,10 +724,231 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AF20E3-EEF9-054E-81C8-86288FFAEC7A}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="C2">
+        <v>0.91</v>
+      </c>
+      <c r="D2">
+        <v>0.95</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0.8</v>
+      </c>
+      <c r="G2">
+        <v>95</v>
+      </c>
+      <c r="H2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="C3">
+        <v>0.88</v>
+      </c>
+      <c r="D3">
+        <v>0.89</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>68</v>
+      </c>
+      <c r="H3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>0.86</v>
+      </c>
+      <c r="D4">
+        <v>0.77</v>
+      </c>
+      <c r="E4">
+        <v>0.5</v>
+      </c>
+      <c r="F4">
+        <v>0.4</v>
+      </c>
+      <c r="G4">
+        <v>50</v>
+      </c>
+      <c r="H4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="D5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E5">
+        <v>0.5</v>
+      </c>
+      <c r="F5">
+        <v>0.1</v>
+      </c>
+      <c r="G5">
+        <v>60</v>
+      </c>
+      <c r="H5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="D6">
+        <v>0.75</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>0.55249999999999999</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>0.25</v>
+      </c>
+      <c r="F7">
+        <v>0.1</v>
+      </c>
+      <c r="G7">
+        <v>108</v>
+      </c>
+      <c r="H7">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.375</v>
+      </c>
+      <c r="C8">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="E8">
+        <v>0.25</v>
+      </c>
+      <c r="F8">
+        <v>0.2</v>
+      </c>
+      <c r="G8">
+        <v>287</v>
+      </c>
+      <c r="H8">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A13592F-7381-2045-A6BB-4532168C020F}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>